<commit_message>
Test-4 results for next year
</commit_message>
<xml_diff>
--- a/migforecasting/less100/tests/test-1.xlsx
+++ b/migforecasting/less100/tests/test-1.xlsx
@@ -45,7 +45,7 @@
     <t>Random Forest-100 (citiesdataset-NYDcor-4.csv) - next year, without dollar</t>
   </si>
   <si>
-    <t>Random Forest-100 (citiesdataset-Dcor-4.csv) - next year, without dollar</t>
+    <t>Random Forest-100 (citiesdataset-Dcor-4.csv) - this year, without dollar</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1462,7 @@
   <dimension ref="C3:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>